<commit_message>
Tweak to example xlsx file
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25756FD9-40DF-46C5-B20F-DAD9354594E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413F906E-9E80-40D7-96D5-BDDCD6FE985A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="-19185" windowWidth="29745" windowHeight="17940" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-33840" yWindow="-16425" windowWidth="29040" windowHeight="15840" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>url</t>
   </si>
@@ -230,13 +230,28 @@
     <t>Need to get this done. Add more teams</t>
   </si>
   <si>
-    <t>Create has to happen before Modify or else it gets ignored.</t>
-  </si>
-  <si>
-    <t>Entries can be in any day order. All those from the one day is picked at a time and executed sequentially in order</t>
-  </si>
-  <si>
-    <t>Add a new tag to collection.</t>
+    <t>Create has to happen before Modify or else it gets ignored</t>
+  </si>
+  <si>
+    <t>Entries can be in any day order. All those from the one day is picked at a time and executed sequentially in order.</t>
+  </si>
+  <si>
+    <t>Add a new tag to collection</t>
+  </si>
+  <si>
+    <t>Remove Parent</t>
+  </si>
+  <si>
+    <t>Business Epic</t>
+  </si>
+  <si>
+    <t>Christmas Release</t>
+  </si>
+  <si>
+    <t>Release 1.3.2</t>
+  </si>
+  <si>
+    <t>Releases</t>
   </si>
 </sst>
 </file>
@@ -281,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -292,9 +307,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -340,7 +356,12 @@
       <sheetData sheetId="3">
         <row r="2">
           <cell r="A2" t="str">
-            <v>1583874351</v>
+            <v>1585036222</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>1585063600</v>
           </cell>
         </row>
       </sheetData>
@@ -648,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E938166-9FC2-447C-B991-15E55C79DF65}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -699,10 +720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,304 +759,369 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="str">
+        <f>'[1]Level 1-0'!A3</f>
+        <v>1585063600</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="6" t="str">
+        <f>'[1]Level 1-0'!A2</f>
+        <v>1585036222</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="4" t="str">
-        <f>'[1]Level 1-0'!A2</f>
-        <v>1583874351</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>4</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5">
-        <v>3</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>2</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="5">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="F17" t="str">
+        <f>IF(ISBLANK('[1]Level 1-0'!A3),0,CONCATENATE("-",'[1]Level 1-0'!A3))</f>
+        <v>-1585063600</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
@@ -1044,8 +1130,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" xr:uid="{F06FD9D9-8D0F-4BC0-AB7C-A79435A049B9}"/>
-    <hyperlink ref="F7" r:id="rId2" xr:uid="{1B90DFCC-0F32-4FD9-9278-318CFE52A877}"/>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{CED0691F-1F96-4931-BD65-5BC9C88E52F3}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{A4FD035D-C0FE-496A-90D4-8508D4FFC063}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1146,19 +1232,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF1A90-24C9-48DD-9C03-23142D45F59E}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="24.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1172,19 +1259,19 @@
         <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1194,17 +1281,35 @@
       <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="E2" s="9">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add note in spreadsheet about Custom Fields
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413F906E-9E80-40D7-96D5-BDDCD6FE985A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18642A30-0A5E-45B7-92DA-6C876F192ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33840" yWindow="-16425" windowWidth="29040" windowHeight="15840" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-3510" yWindow="-22635" windowWidth="33675" windowHeight="16725" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>url</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>Releases</t>
+  </si>
+  <si>
+    <t>WSJF</t>
+  </si>
+  <si>
+    <t>Custom Fields on a board are checked if it is not a standard Card field. If still no match, then it is ignored</t>
   </si>
 </sst>
 </file>
@@ -669,7 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E938166-9FC2-447C-B991-15E55C79DF65}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -720,10 +726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,6 +1127,29 @@
       <c r="G17" s="2"/>
       <c r="H17" s="4" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18">
+        <v>3.1415899999999999</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a couple more fields
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18642A30-0A5E-45B7-92DA-6C876F192ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A9AB8C-AF6E-41FD-B119-4DB47C199CF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3510" yWindow="-22635" windowWidth="33675" windowHeight="16725" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-30" yWindow="-22365" windowWidth="28770" windowHeight="15600" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t>url</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Value2</t>
   </si>
   <si>
-    <t>Move a card to a new lane and use Value2 as wipOverrideComment</t>
-  </si>
-  <si>
     <t>Need to get this done. Add more teams</t>
   </si>
   <si>
@@ -257,7 +254,31 @@
     <t>WSJF</t>
   </si>
   <si>
-    <t>Custom Fields on a board are checked if it is not a standard Card field. If still no match, then it is ignored</t>
+    <t>externalLink</t>
+  </si>
+  <si>
+    <t>My GitHub</t>
+  </si>
+  <si>
+    <t>https://github.com/nikantonelli/GroundHog</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>Reposition cards in their lane</t>
+  </si>
+  <si>
+    <t>It will never get to day 99 if Config-&gt;cyclelength = 14. To run just this one, you could use the commandline options: -f &lt;file&gt; -u 0 -b 99</t>
+  </si>
+  <si>
+    <t>Custom Fields on a board are checked if it is not a standard Card field. If still no match, then it is ignored. Numbers are to 4 decimal places and get rounded (e.g 3.1416)</t>
+  </si>
+  <si>
+    <t>Move a card to a new lane and use Value2 as wipOverrideComment, if needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple Parents </t>
   </si>
 </sst>
 </file>
@@ -359,18 +380,7 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>1585036222</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>1585063600</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -726,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +789,7 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -797,7 +807,7 @@
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -815,7 +825,7 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -839,7 +849,7 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -880,9 +890,9 @@
       <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7">
         <f>'[1]Level 1-0'!A3</f>
-        <v>1585063600</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
@@ -905,13 +915,13 @@
       <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="6" t="str">
+      <c r="F8" s="6">
         <f>'[1]Level 1-0'!A2</f>
-        <v>1585036222</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1026,10 +1036,10 @@
         <v>39</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1120,13 +1130,13 @@
       <c r="E17" t="s">
         <v>36</v>
       </c>
-      <c r="F17" t="str">
+      <c r="F17">
         <f>IF(ISBLANK('[1]Level 1-0'!A3),0,CONCATENATE("-",'[1]Level 1-0'!A3))</f>
-        <v>-1585063600</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1143,13 +1153,85 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18">
         <v>3.1415899999999999</v>
       </c>
       <c r="H18" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>99</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" t="s">
         <v>72</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1161,9 +1243,10 @@
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" xr:uid="{CED0691F-1F96-4931-BD65-5BC9C88E52F3}"/>
     <hyperlink ref="F9" r:id="rId2" xr:uid="{A4FD035D-C0FE-496A-90D4-8508D4FFC063}"/>
+    <hyperlink ref="G20" r:id="rId3" xr:uid="{371591A7-8DB5-418C-85F9-1F02F443F075}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1325,16 +1408,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some tidy up tweaks.
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADD5A0D-BC7A-408B-8306-FE75099E61FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DC7CCF-E4DB-4C76-8470-C88B5D3C31E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="600" windowWidth="28770" windowHeight="15600" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="2520" yWindow="-16710" windowWidth="28770" windowHeight="15600" activeTab="2" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -374,10 +374,21 @@
       <sheetName val="Level 1-0"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v/>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -735,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -887,9 +898,9 @@
       <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="str">
         <f>'[1]Level 1-0'!A3</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
@@ -912,9 +923,9 @@
       <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="6" t="str">
         <f>'[1]Level 1-0'!A2</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
@@ -1127,9 +1138,9 @@
       <c r="E17" t="s">
         <v>36</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="str">
         <f>IF(ISBLANK('[1]Level 1-0'!A3),0,CONCATENATE("-",'[1]Level 1-0'!A3))</f>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="4" t="s">
@@ -1251,7 +1262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525ADE1B-52CA-4A24-AFEE-91E8EE2AC7BD}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Move value1 and 2 to single comma separated string
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DC7CCF-E4DB-4C76-8470-C88B5D3C31E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87CCBE8-3A00-4646-9B26-D25303D42F81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="-16710" windowWidth="28770" windowHeight="15600" activeTab="2" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-5040" yWindow="-24120" windowWidth="38640" windowHeight="23640" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>url</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Implementation per ART/VS|Cross-ART|In Progress</t>
   </si>
   <si>
-    <t>Funding</t>
-  </si>
-  <si>
     <t>-Current Sprint</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Remove isBlocked by clearing blockedReason with a "-"</t>
-  </si>
-  <si>
     <t>Child lane names separated by "|"</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>Value2</t>
   </si>
   <si>
-    <t>Need to get this done. Add more teams</t>
-  </si>
-  <si>
     <t>Create has to happen before Modify or else it gets ignored</t>
   </si>
   <si>
@@ -233,12 +224,6 @@
     <t>externalLink</t>
   </si>
   <si>
-    <t>My GitHub</t>
-  </si>
-  <si>
-    <t>https://github.com/nikantonelli/GroundHog</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -251,9 +236,6 @@
     <t>Custom Fields on a board are checked if it is not a standard Card field. If still no match, then it is ignored. Numbers are to 4 decimal places and get rounded (e.g 3.1416)</t>
   </si>
   <si>
-    <t>Move a card to a new lane and use Value2 as wipOverrideComment, if needed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Multiple Parents </t>
   </si>
   <si>
@@ -264,6 +246,21 @@
   </si>
   <si>
     <t>These entries are referred to in the Changes sheet. Add more fields to the right for setting fields on card  creation. Fields name must  match the API or be CustomFields. Fields that start with a capital letter are treated to special transformations</t>
+  </si>
+  <si>
+    <t>Remove isBlocked by starting blockReason with a "-", or by setting it to: "" or single char entry</t>
+  </si>
+  <si>
+    <t>My GitHub, https://github.com/nikantonelli/GroundHog</t>
+  </si>
+  <si>
+    <t>Code looks for last occurence of "," to separate url</t>
+  </si>
+  <si>
+    <t>Funding,Need to get this done. Add more teams</t>
+  </si>
+  <si>
+    <t>Move a card to a new lane and use string after first ","  as wipOverrideComment, if needed</t>
   </si>
 </sst>
 </file>
@@ -731,7 +728,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -746,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,10 +772,10 @@
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H1" s="5"/>
     </row>
@@ -797,7 +794,7 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -815,7 +812,7 @@
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -833,7 +830,7 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -857,7 +854,7 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -904,7 +901,7 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,7 +926,7 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -953,7 +950,7 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1021,7 +1018,7 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1041,13 +1038,11 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>53</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1067,11 +1062,11 @@
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,14 +1083,14 @@
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1112,14 +1107,14 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="4" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1144,7 +1139,7 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1161,13 +1156,13 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F18">
         <v>3.1415899999999999</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1187,11 +1182,11 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1208,15 +1203,15 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1232,14 +1227,14 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1251,10 +1246,9 @@
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" xr:uid="{CED0691F-1F96-4931-BD65-5BC9C88E52F3}"/>
     <hyperlink ref="F9" r:id="rId2" xr:uid="{A4FD035D-C0FE-496A-90D4-8508D4FFC063}"/>
-    <hyperlink ref="G20" r:id="rId3" xr:uid="{371591A7-8DB5-418C-85F9-1F02F443F075}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1262,7 +1256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525ADE1B-52CA-4A24-AFEE-91E8EE2AC7BD}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -1303,19 +1297,19 @@
     </row>
     <row r="2" spans="1:9" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1408,16 +1402,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes to excel spreadsheet example
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87CCBE8-3A00-4646-9B26-D25303D42F81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D101E9E-DEAD-4033-8750-0E57FA57A396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5040" yWindow="-24120" windowWidth="38640" windowHeight="23640" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-2970" yWindow="-20940" windowWidth="32910" windowHeight="16485" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
   <si>
     <t>url</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>Move a card to a new lane and use string after first ","  as wipOverrideComment, if needed</t>
+  </si>
+  <si>
+    <t>critical</t>
+  </si>
+  <si>
+    <t>Use lowercase value - NOT what you see in the UI.</t>
   </si>
 </sst>
 </file>
@@ -337,7 +343,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -741,10 +757,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,8 +1253,37 @@
         <v>62</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C21 C23:C1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix lane finding in multiple-child lane
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DC7CCF-E4DB-4C76-8470-C88B5D3C31E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79F9532-FE10-47E2-8E6F-A26AA555FA69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="-16710" windowWidth="28770" windowHeight="15600" activeTab="2" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15570" activeTab="3" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>Implementation per ART/VS|Cross-ART|In Progress</t>
   </si>
   <si>
-    <t>Funding</t>
-  </si>
-  <si>
     <t>-Current Sprint</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>Value2</t>
   </si>
   <si>
-    <t>Need to get this done. Add more teams</t>
-  </si>
-  <si>
     <t>Create has to happen before Modify or else it gets ignored</t>
   </si>
   <si>
@@ -233,12 +227,6 @@
     <t>externalLink</t>
   </si>
   <si>
-    <t>My GitHub</t>
-  </si>
-  <si>
-    <t>https://github.com/nikantonelli/GroundHog</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -251,19 +239,31 @@
     <t>Custom Fields on a board are checked if it is not a standard Card field. If still no match, then it is ignored. Numbers are to 4 decimal places and get rounded (e.g 3.1416)</t>
   </si>
   <si>
-    <t>Move a card to a new lane and use Value2 as wipOverrideComment, if needed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Multiple Parents </t>
   </si>
   <si>
-    <t>Lane lookup is done using the '|' or '&amp;' character as separator for child lanes</t>
-  </si>
-  <si>
     <t>Fields you cannot put in the creation are those that require two parameters. The ones you will have problems with are: Lanes that have a WIPLimit set, externalLink. To get around this problem, do a create first and then add a Modify line to the Changes sheet (which can handle Value1,Value2 pairs.</t>
   </si>
   <si>
     <t>These entries are referred to in the Changes sheet. Add more fields to the right for setting fields on card  creation. Fields name must  match the API or be CustomFields. Fields that start with a capital letter are treated to special transformations</t>
+  </si>
+  <si>
+    <t>Lane lookup is done using the '|' or '&amp;' character as separator for child lanes. If you need to add an overrideWipComment, then add a phrase after a comma</t>
+  </si>
+  <si>
+    <t>Analysis, Override my wip</t>
+  </si>
+  <si>
+    <t>Funding, Need to get this done. Add more teams</t>
+  </si>
+  <si>
+    <t>Move a card to a new lane and put overrideWipComment, if needed, after a comma</t>
+  </si>
+  <si>
+    <t>My GitHub, https://github.com/nikantonelli/GroundHog</t>
+  </si>
+  <si>
+    <t>Put label first - BUT must not contain any comma chars.</t>
   </si>
 </sst>
 </file>
@@ -374,18 +374,13 @@
       <sheetName val="Level 1-0"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="2">
           <cell r="A2" t="str">
-            <v/>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v/>
+            <v>1588096724</v>
           </cell>
         </row>
       </sheetData>
@@ -731,7 +726,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -747,7 +742,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,10 +770,10 @@
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="H1" s="5"/>
     </row>
@@ -797,7 +792,7 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -815,7 +810,7 @@
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -833,7 +828,7 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -857,7 +852,7 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -898,13 +893,13 @@
       <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7">
         <f>'[1]Level 1-0'!A3</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,11 +920,11 @@
       </c>
       <c r="F8" s="6" t="str">
         <f>'[1]Level 1-0'!A2</f>
-        <v/>
+        <v>1588096724</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -953,7 +948,7 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1021,7 +1016,7 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1041,13 +1036,11 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>53</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1067,11 +1060,11 @@
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,14 +1081,14 @@
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1112,14 +1105,14 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1138,13 +1131,13 @@
       <c r="E17" t="s">
         <v>36</v>
       </c>
-      <c r="F17" t="str">
+      <c r="F17">
         <f>IF(ISBLANK('[1]Level 1-0'!A3),0,CONCATENATE("-",'[1]Level 1-0'!A3))</f>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1161,13 +1154,13 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F18">
         <v>3.1415899999999999</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1187,11 +1180,11 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1208,15 +1201,15 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1232,14 +1225,14 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1251,19 +1244,18 @@
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" xr:uid="{CED0691F-1F96-4931-BD65-5BC9C88E52F3}"/>
     <hyperlink ref="F9" r:id="rId2" xr:uid="{A4FD035D-C0FE-496A-90D4-8508D4FFC063}"/>
-    <hyperlink ref="G20" r:id="rId3" xr:uid="{371591A7-8DB5-418C-85F9-1F02F443F075}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525ADE1B-52CA-4A24-AFEE-91E8EE2AC7BD}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,19 +1295,19 @@
     </row>
     <row r="2" spans="1:9" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1334,6 +1326,11 @@
       </c>
       <c r="H3" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1346,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF1A90-24C9-48DD-9C03-23142D45F59E}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1408,16 +1405,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add few more debug messages
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79F9532-FE10-47E2-8E6F-A26AA555FA69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BADB56-7443-4FDA-8296-DDEA51EFFB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15570" activeTab="3" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-5040" yWindow="-24120" windowWidth="38640" windowHeight="23640" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>url</t>
   </si>
@@ -191,12 +191,6 @@
     <t>blockReason</t>
   </si>
   <si>
-    <t>Value1</t>
-  </si>
-  <si>
-    <t>Value2</t>
-  </si>
-  <si>
     <t>Create has to happen before Modify or else it gets ignored</t>
   </si>
   <si>
@@ -264,6 +258,9 @@
   </si>
   <si>
     <t>Put label first - BUT must not contain any comma chars.</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -308,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -321,7 +318,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -381,6 +377,11 @@
         <row r="2">
           <cell r="A2" t="str">
             <v>1588096724</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>1588608850</v>
           </cell>
         </row>
       </sheetData>
@@ -739,21 +740,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="27.5703125" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="50.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="41.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="86.85546875" customWidth="1"/>
+    <col min="7" max="7" width="86.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -770,14 +770,11 @@
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -790,12 +787,11 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -808,12 +804,11 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -826,12 +821,11 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -850,12 +844,11 @@
       <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -874,10 +867,9 @@
       <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -893,16 +885,15 @@
       <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="str">
         <f>'[1]Level 1-0'!A3</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4" t="s">
+        <v>1588608850</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -922,12 +913,11 @@
         <f>'[1]Level 1-0'!A2</f>
         <v>1588096724</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -946,12 +936,11 @@
       <c r="F9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -970,10 +959,9 @@
       <c r="F10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -992,10 +980,9 @@
       <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1014,12 +1001,11 @@
       <c r="F12" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1036,14 +1022,13 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1062,12 +1047,11 @@
       <c r="F14" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1086,12 +1070,11 @@
       <c r="F15" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1110,12 +1093,11 @@
       <c r="F16" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1131,16 +1113,15 @@
       <c r="E17" t="s">
         <v>36</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="str">
         <f>IF(ISBLANK('[1]Level 1-0'!A3),0,CONCATENATE("-",'[1]Level 1-0'!A3))</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>-1588608850</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1154,16 +1135,16 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F18">
         <v>3.1415899999999999</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G18" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>99</v>
       </c>
@@ -1180,14 +1161,13 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1201,17 +1181,16 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1225,14 +1204,13 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="4" t="s">
-        <v>63</v>
+      <c r="G21" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1293,25 +1271,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11" t="s">
+    <row r="2" spans="1:9" s="10" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1330,7 +1308,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1343,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF1A90-24C9-48DD-9C03-23142D45F59E}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1351,7 +1329,7 @@
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1" collapsed="1"/>
     <col min="2" max="4" width="24.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5703125" style="8" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
@@ -1370,7 +1348,7 @@
       <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F1" t="s">
@@ -1393,7 +1371,7 @@
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1405,16 +1383,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge updates form GroundHog
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D101E9E-DEAD-4033-8750-0E57FA57A396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED80E0B-DD1E-4677-A6EB-1F6FFE980175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2970" yWindow="-20940" windowWidth="32910" windowHeight="16485" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
   <si>
     <t>url</t>
   </si>
@@ -188,12 +188,6 @@
     <t>blockReason</t>
   </si>
   <si>
-    <t>Value1</t>
-  </si>
-  <si>
-    <t>Value2</t>
-  </si>
-  <si>
     <t>Create has to happen before Modify or else it gets ignored</t>
   </si>
   <si>
@@ -267,6 +261,9 @@
   </si>
   <si>
     <t>Use lowercase value - NOT what you see in the UI.</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -311,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -324,7 +321,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -757,21 +753,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="27.5703125" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="50.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="41.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="86.85546875" customWidth="1"/>
+    <col min="7" max="7" width="86.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -788,14 +783,11 @@
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -808,12 +800,11 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -826,12 +817,11 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -844,12 +834,11 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -868,12 +857,11 @@
       <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -892,10 +880,9 @@
       <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -915,12 +902,11 @@
         <f>'[1]Level 1-0'!A3</f>
         <v/>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -940,12 +926,11 @@
         <f>'[1]Level 1-0'!A2</f>
         <v/>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -964,12 +949,11 @@
       <c r="F9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -988,10 +972,9 @@
       <c r="F10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1010,10 +993,9 @@
       <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1032,12 +1014,11 @@
       <c r="F12" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1054,14 +1035,13 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1080,12 +1060,11 @@
       <c r="F14" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1104,12 +1083,11 @@
       <c r="F15" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1128,12 +1106,11 @@
       <c r="F16" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1153,12 +1130,11 @@
         <f>IF(ISBLANK('[1]Level 1-0'!A3),0,CONCATENATE("-",'[1]Level 1-0'!A3))</f>
         <v>-</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G17" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1172,16 +1148,16 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F18">
         <v>3.1415899999999999</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G18" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>99</v>
       </c>
@@ -1198,14 +1174,13 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1219,17 +1194,16 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1243,17 +1217,16 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1270,11 +1243,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1340,25 +1312,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
+    <row r="2" spans="1:9" s="10" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11" t="s">
-        <v>67</v>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1393,7 +1365,7 @@
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1" collapsed="1"/>
     <col min="2" max="4" width="24.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5703125" style="8" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
@@ -1412,7 +1384,7 @@
       <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F1" t="s">
@@ -1435,7 +1407,7 @@
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1447,16 +1419,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small update to example spreadsheet
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED80E0B-DD1E-4677-A6EB-1F6FFE980175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD36F33-25E0-44FB-A082-AC6EB5B8C396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="3060" yWindow="-19395" windowWidth="28845" windowHeight="15870" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>Analysis</t>
   </si>
   <si>
-    <t>needYourApiKeyOrYouUsernamePasswordPair</t>
-  </si>
-  <si>
     <t>My Scheduled Story</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>needYourApiKeyOrYourUsernamePasswordPair</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,13 +734,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="E2">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -783,7 +783,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -801,7 +801,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -818,7 +818,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -835,7 +835,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -852,13 +852,13 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -878,7 +878,7 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -896,14 +896,14 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" t="str">
         <f>'[1]Level 1-0'!A3</f>
         <v/>
       </c>
       <c r="G7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -920,14 +920,14 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="6" t="str">
         <f>'[1]Level 1-0'!A2</f>
         <v/>
       </c>
       <c r="G8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -947,10 +947,10 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -1012,10 +1012,10 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1035,10 +1035,10 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1055,13 +1055,13 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,13 +1078,13 @@
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1101,13 +1101,13 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1124,14 +1124,14 @@
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" t="str">
         <f>IF(ISBLANK('[1]Level 1-0'!A3),0,CONCATENATE("-",'[1]Level 1-0'!A3))</f>
         <v>-</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1148,13 +1148,13 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18">
         <v>3.1415899999999999</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1174,10 +1174,10 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1194,13 +1194,13 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1217,13 +1217,13 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1243,10 +1243,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1314,19 +1314,19 @@
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1341,10 +1341,10 @@
         <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1405,13 +1405,13 @@
         <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="8">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1419,16 +1419,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove daft Excel reference to external file
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BADB56-7443-4FDA-8296-DDEA51EFFB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5502A9DC-67A3-4082-8157-731D8DDE8546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5040" yWindow="-24120" windowWidth="38640" windowHeight="23640" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-4335" yWindow="-21990" windowWidth="34125" windowHeight="17235" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="Level 0-0" sheetId="3" r:id="rId3"/>
     <sheet name="Level 1-0" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -358,36 +355,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Config"/>
-      <sheetName val="Changes"/>
-      <sheetName val="Level 0-0"/>
-      <sheetName val="Level 1-0"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>1588096724</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>1588608850</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -743,7 +710,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,9 +852,9 @@
       <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="str">
-        <f>'[1]Level 1-0'!A3</f>
-        <v>1588608850</v>
+      <c r="F7">
+        <f>'Level 1-0'!A3</f>
+        <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>47</v>
@@ -909,9 +876,9 @@
       <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="6" t="str">
-        <f>'[1]Level 1-0'!A2</f>
-        <v>1588096724</v>
+      <c r="F8" s="6">
+        <f>'Level 1-0'!A2</f>
+        <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>64</v>
@@ -1113,9 +1080,9 @@
       <c r="E17" t="s">
         <v>36</v>
       </c>
-      <c r="F17" t="str">
-        <f>IF(ISBLANK('[1]Level 1-0'!A3),0,CONCATENATE("-",'[1]Level 1-0'!A3))</f>
-        <v>-1588608850</v>
+      <c r="F17">
+        <f>IF(ISBLANK('Level 1-0'!A3),0,CONCATENATE("-",'Level 1-0'!A3))</f>
+        <v>0</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Add in a line for attachments
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5502A9DC-67A3-4082-8157-731D8DDE8546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC88BF66-407F-446C-B0BC-7B40FEA8DC4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4335" yWindow="-21990" windowWidth="34125" windowHeight="17235" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-33285" yWindow="-14970" windowWidth="25590" windowHeight="11490" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
   <si>
     <t>url</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>attachments</t>
+  </si>
+  <si>
+    <t>MyFilename.txt</t>
+  </si>
+  <si>
+    <t>Add this file as an attachment to this card. The full path of the file is needed if not specified in your env variables</t>
   </si>
 </sst>
 </file>
@@ -707,10 +716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,6 +1187,29 @@
       </c>
       <c r="G21" s="4" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update example spreadsheet with more entries
</commit_message>
<xml_diff>
--- a/Scrum Teams_example.xlsx
+++ b/Scrum Teams_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Groundhog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC88BF66-407F-446C-B0BC-7B40FEA8DC4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D0CCCF-DAB1-4567-B3EE-9687335DB5BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33285" yWindow="-14970" windowWidth="25590" windowHeight="11490" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
   <si>
     <t>url</t>
   </si>
@@ -167,12 +167,6 @@
     <t>Set isBlocked by providing a blockedReason</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Remove isBlocked by clearing blockedReason with a "-"</t>
-  </si>
-  <si>
     <t>Child lane names separated by "|"</t>
   </si>
   <si>
@@ -267,6 +261,30 @@
   </si>
   <si>
     <t>Add this file as an attachment to this card. The full path of the file is needed if not specified in your env variables</t>
+  </si>
+  <si>
+    <t>customIcon</t>
+  </si>
+  <si>
+    <t>Regulatory</t>
+  </si>
+  <si>
+    <t>Add the name of the Icon here</t>
+  </si>
+  <si>
+    <t>-Test System Back Up</t>
+  </si>
+  <si>
+    <t>Remove isBlocked by clearing blockedReason with an empty cell</t>
+  </si>
+  <si>
+    <t>Remove isBlocked by clearing blockedReason with a "-" and adds the comment</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Add a priority with the name</t>
   </si>
 </sst>
 </file>
@@ -342,7 +360,37 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -703,7 +751,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -716,10 +764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8163DD46-63A6-4C19-A83F-CE88989C762C}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +794,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -764,7 +812,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -781,7 +829,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -798,7 +846,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -821,7 +869,7 @@
         <v>34</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -866,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -890,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -913,7 +961,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -978,7 +1026,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -998,10 +1046,10 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1029,7 +1077,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1041,7 +1089,7 @@
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
         <v>41</v>
@@ -1052,7 +1100,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -1064,13 +1112,11 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" t="s">
-        <v>43</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F16" s="6"/>
       <c r="G16" s="4" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1087,83 +1133,83 @@
         <v>21</v>
       </c>
       <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
         <v>36</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <f>IF(ISBLANK('Level 1-0'!A3),0,CONCATENATE("-",'Level 1-0'!A3))</f>
         <v>0</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18">
-        <v>3.1415899999999999</v>
-      </c>
       <c r="G18" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19">
+        <v>3.1415899999999999</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>99</v>
       </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
         <v>14</v>
       </c>
-      <c r="F19" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>59</v>
-      </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1180,40 +1226,124 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>0</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>5</v>
       </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F22" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="F24" t="s">
         <v>76</v>
       </c>
+      <c r="G24" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C16 C26:C1048576 C18:C23">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -1272,19 +1402,19 @@
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1307,7 +1437,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1382,16 +1512,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>